<commit_message>
Running on Mac Studio
</commit_message>
<xml_diff>
--- a/results/0927/2022-0927_resnet34_malmotest.xlsx
+++ b/results/0927/2022-0927_resnet34_malmotest.xlsx
@@ -511,7 +511,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>IP</t>
+          <t>complete</t>
         </is>
       </c>
       <c r="C2" t="n">
@@ -545,27 +545,27 @@
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>[81, 104]</t>
+          <t>[81, 91]</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>[0.086, 0.085]</t>
+          <t>[0.086, 0.086]</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>[0, 30]</t>
+          <t>[0, 5]</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>[0, 11.199999999999976]</t>
+          <t>[0, 2.3000000000000007]</t>
         </is>
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>[0, 0.12]</t>
+          <t>[0, 0.1]</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
@@ -578,553 +578,153 @@
       <c r="A3" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>IP</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>1</v>
-      </c>
-      <c r="D3" t="n">
-        <v>1</v>
-      </c>
-      <c r="E3" t="n">
-        <v>0</v>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>grocery</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>classWt</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>SVM</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>['0_0']</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>[81, 111]</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>[0.342, 0.37]</t>
-        </is>
-      </c>
-      <c r="L3" t="inlineStr">
-        <is>
-          <t>[0, 30]</t>
-        </is>
-      </c>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t>[0, 10.899999999999977]</t>
-        </is>
-      </c>
-      <c r="N3" t="inlineStr">
-        <is>
-          <t>[0, 0.02]</t>
-        </is>
-      </c>
-      <c r="O3" t="inlineStr">
-        <is>
-          <t>[0, -10, -10, 0, -10, -10, -10, -10, -10, -10, 0, -10, 0, -10, -10, -10, -20, -20, -20, 0, -20, 0, -20, 0, -20, -20, 0, -20, 0, -20, 0, 0, -20, -20, -20, 0, -20, 0, 0, -20, -10, -20, -20, -20, -20, -10, -20, -10, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, -10, 0, 0, -10, -10, -10, 0, 0, 0, -10, 0, 0, 0, 0, 0, 0, -20]</t>
-        </is>
-      </c>
+      <c r="B3" t="inlineStr"/>
+      <c r="C3" t="inlineStr"/>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="inlineStr"/>
+      <c r="J3" t="inlineStr"/>
+      <c r="K3" t="inlineStr"/>
+      <c r="L3" t="inlineStr"/>
+      <c r="M3" t="inlineStr"/>
+      <c r="N3" t="inlineStr"/>
+      <c r="O3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>IP</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>2</v>
-      </c>
-      <c r="D4" t="n">
-        <v>1</v>
-      </c>
-      <c r="E4" t="n">
-        <v>0</v>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>grocery</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>random</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>WVS</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>['0_0']</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>[81, 115]</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>[0.086, 0.085]</t>
-        </is>
-      </c>
-      <c r="L4" t="inlineStr">
-        <is>
-          <t>[0, 30]</t>
-        </is>
-      </c>
-      <c r="M4" t="inlineStr">
-        <is>
-          <t>[0, 11.499999999999975]</t>
-        </is>
-      </c>
-      <c r="N4" t="inlineStr">
-        <is>
-          <t>[0, 0.12]</t>
-        </is>
-      </c>
-      <c r="O4" t="inlineStr">
-        <is>
-          <t>[0, 0, 0, 0, -20, 0, 0, -10, 0, 0, -10, -10, 0, -10, 0, -20, -10, 0, 0, 0, -20, -10, -10, 0, -20, -20, 0, -20, 0, -20, -20, 0, 0, 0, -10, 0, 0, -10, -10, -20, 0, 0, -10, -20, -10, -10, -10, 0, -20, 0, 0, -20, 0, 0, -10, -20, 0, -10, -20, 0, 0, -20, 0, -10, 0, 0, 0, -20, -10, 0, -10, 0, -20, 0, -10, -20, -20, 0, -20, 0, 0]</t>
-        </is>
-      </c>
+      <c r="B4" t="inlineStr"/>
+      <c r="C4" t="inlineStr"/>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr"/>
+      <c r="J4" t="inlineStr"/>
+      <c r="K4" t="inlineStr"/>
+      <c r="L4" t="inlineStr"/>
+      <c r="M4" t="inlineStr"/>
+      <c r="N4" t="inlineStr"/>
+      <c r="O4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>IP</t>
-        </is>
-      </c>
-      <c r="C5" t="n">
-        <v>3</v>
-      </c>
-      <c r="D5" t="n">
-        <v>1</v>
-      </c>
-      <c r="E5" t="n">
-        <v>0</v>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>grocery</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>random</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>SVM</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>['0_0']</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>[81, 118]</t>
-        </is>
-      </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>[0.342, 0.367]</t>
-        </is>
-      </c>
-      <c r="L5" t="inlineStr">
-        <is>
-          <t>[0, 30]</t>
-        </is>
-      </c>
-      <c r="M5" t="inlineStr">
-        <is>
-          <t>[0, 11.099999999999977]</t>
-        </is>
-      </c>
-      <c r="N5" t="inlineStr">
-        <is>
-          <t>[0, 0.02]</t>
-        </is>
-      </c>
-      <c r="O5" t="inlineStr">
-        <is>
-          <t>[0, 0, 0, 0, -20, 0, 0, -10, 0, 0, -10, -10, 0, -10, 0, -20, -10, 0, 0, 0, -20, -10, -10, 0, -20, -20, 0, -20, 0, -20, -20, 0, 0, 0, -10, 0, 0, -10, -10, -20, 0, 0, -10, -20, -10, -10, -10, 0, -20, 0, 0, -20, 0, 0, -10, -20, 0, -10, -20, 0, 0, -20, 0, -10, 0, 0, 0, -20, -10, 0, -10, 0, -20, 0, -10, -20, -20, 0, -20, 0, 0]</t>
-        </is>
-      </c>
+      <c r="B5" t="inlineStr"/>
+      <c r="C5" t="inlineStr"/>
+      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="inlineStr"/>
+      <c r="F5" t="inlineStr"/>
+      <c r="G5" t="inlineStr"/>
+      <c r="H5" t="inlineStr"/>
+      <c r="I5" t="inlineStr"/>
+      <c r="J5" t="inlineStr"/>
+      <c r="K5" t="inlineStr"/>
+      <c r="L5" t="inlineStr"/>
+      <c r="M5" t="inlineStr"/>
+      <c r="N5" t="inlineStr"/>
+      <c r="O5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>IP</t>
-        </is>
-      </c>
-      <c r="C6" t="n">
-        <v>4</v>
-      </c>
-      <c r="D6" t="n">
-        <v>1</v>
-      </c>
-      <c r="E6" t="n">
-        <v>0</v>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>cifar</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>classWt</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>WVS</t>
-        </is>
-      </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>['0_0']</t>
-        </is>
-      </c>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>[100, 124]</t>
-        </is>
-      </c>
-      <c r="K6" t="inlineStr">
-        <is>
-          <t>[0.012, 0.01]</t>
-        </is>
-      </c>
-      <c r="L6" t="inlineStr">
-        <is>
-          <t>[0, 30]</t>
-        </is>
-      </c>
-      <c r="M6" t="inlineStr">
-        <is>
-          <t>[0, 11.399999999999975]</t>
-        </is>
-      </c>
-      <c r="N6" t="inlineStr">
-        <is>
-          <t>[0, 1.42]</t>
-        </is>
-      </c>
-      <c r="O6" t="inlineStr">
-        <is>
-          <t>[-20, 0, -10, -10, -10, 0, 0, 0, 0, 0, -20, -20, 0, -20, 0, -20, 0, 0, -20, 0, -10, 0, -20, 0, 0, -20, -20, -10, -10, -10, -10, -10, -10, -10, -10, -10, -10, -10, -20, -20, -20, 0, 0, 0, -20, -20, -20, -20, 0, 0, -20, -20, -20, -20, -20, -20, 0, -20, -20, -20, -10, 0, -10, -10, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, -10, -10, -10, 0, -10, 0, 0, -10, -10, -10, 0, 0, 0, 0, 0, 0, 0, 0]</t>
-        </is>
-      </c>
+      <c r="B6" t="inlineStr"/>
+      <c r="C6" t="inlineStr"/>
+      <c r="D6" t="inlineStr"/>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="inlineStr"/>
+      <c r="G6" t="inlineStr"/>
+      <c r="H6" t="inlineStr"/>
+      <c r="I6" t="inlineStr"/>
+      <c r="J6" t="inlineStr"/>
+      <c r="K6" t="inlineStr"/>
+      <c r="L6" t="inlineStr"/>
+      <c r="M6" t="inlineStr"/>
+      <c r="N6" t="inlineStr"/>
+      <c r="O6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>IP</t>
-        </is>
-      </c>
-      <c r="C7" t="n">
-        <v>5</v>
-      </c>
-      <c r="D7" t="n">
-        <v>1</v>
-      </c>
-      <c r="E7" t="n">
-        <v>0</v>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>cifar</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>classWt</t>
-        </is>
-      </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>SVM</t>
-        </is>
-      </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>['0_0']</t>
-        </is>
-      </c>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>[100, 101]</t>
-        </is>
-      </c>
-      <c r="K7" t="inlineStr">
-        <is>
-          <t>[0.198, 0.197]</t>
-        </is>
-      </c>
-      <c r="L7" t="inlineStr">
-        <is>
-          <t>[0, 30]</t>
-        </is>
-      </c>
-      <c r="M7" t="inlineStr">
-        <is>
-          <t>[0, 13.499999999999968]</t>
-        </is>
-      </c>
-      <c r="N7" t="inlineStr">
-        <is>
-          <t>[0, 0.18]</t>
-        </is>
-      </c>
-      <c r="O7" t="inlineStr">
-        <is>
-          <t>[-20, 0, -10, -10, -10, 0, 0, 0, 0, 0, -20, -20, 0, -20, 0, -20, 0, 0, -20, 0, -10, 0, -20, 0, 0, -20, -20, -10, -10, -10, -10, -10, -10, -10, -10, -10, -10, -10, -20, -20, -20, 0, 0, 0, -20, -20, -20, -20, 0, 0, -20, -20, -20, -20, -20, -20, 0, -20, -20, -20, -10, 0, -10, -10, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, -10, -10, -10, 0, -10, 0, 0, -10, -10, -10, 0, 0, 0, 0, 0, 0, 0, 0]</t>
-        </is>
-      </c>
+      <c r="B7" t="inlineStr"/>
+      <c r="C7" t="inlineStr"/>
+      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="inlineStr"/>
+      <c r="F7" t="inlineStr"/>
+      <c r="G7" t="inlineStr"/>
+      <c r="H7" t="inlineStr"/>
+      <c r="I7" t="inlineStr"/>
+      <c r="J7" t="inlineStr"/>
+      <c r="K7" t="inlineStr"/>
+      <c r="L7" t="inlineStr"/>
+      <c r="M7" t="inlineStr"/>
+      <c r="N7" t="inlineStr"/>
+      <c r="O7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>IP</t>
-        </is>
-      </c>
-      <c r="C8" t="n">
-        <v>6</v>
-      </c>
-      <c r="D8" t="n">
-        <v>1</v>
-      </c>
-      <c r="E8" t="n">
-        <v>0</v>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>cifar</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>random</t>
-        </is>
-      </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>WVS</t>
-        </is>
-      </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>['0_0']</t>
-        </is>
-      </c>
-      <c r="J8" t="inlineStr">
-        <is>
-          <t>[100, 136]</t>
-        </is>
-      </c>
-      <c r="K8" t="inlineStr">
-        <is>
-          <t>[0.012, 0.006]</t>
-        </is>
-      </c>
-      <c r="L8" t="inlineStr">
-        <is>
-          <t>[0, 30]</t>
-        </is>
-      </c>
-      <c r="M8" t="inlineStr">
-        <is>
-          <t>[0, 12.99999999999997]</t>
-        </is>
-      </c>
-      <c r="N8" t="inlineStr">
-        <is>
-          <t>[0, 1.48]</t>
-        </is>
-      </c>
-      <c r="O8" t="inlineStr">
-        <is>
-          <t>[-10, -20, 0, -10, -10, 0, -20, 0, 0, -20, 0, 0, -10, -20, 0, -10, -20, 0, 0, -20, 0, -10, 0, 0, 0, -20, -10, 0, -10, 0, -20, 0, -10, -20, -10, 0, -20, 0, 0, -20, 0, -20, 0, 0, -10, 0, -20, 0, 0, 0, 0, -20, -10, 0, -20, -20, -10, -10, 0, 0, -20, -10, 0, -20, -20, -20, 0, 0, -10, 0, 0, -20, 0, -10, -10, -10, -10, -10, -20, 0, 0, -10, 0, 0, -10, 0, 0, 0, -10, -20, 0, -20, 0, 0, 0, -20, -10, 0, 0, 0]</t>
-        </is>
-      </c>
+      <c r="B8" t="inlineStr"/>
+      <c r="C8" t="inlineStr"/>
+      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="inlineStr"/>
+      <c r="F8" t="inlineStr"/>
+      <c r="G8" t="inlineStr"/>
+      <c r="H8" t="inlineStr"/>
+      <c r="I8" t="inlineStr"/>
+      <c r="J8" t="inlineStr"/>
+      <c r="K8" t="inlineStr"/>
+      <c r="L8" t="inlineStr"/>
+      <c r="M8" t="inlineStr"/>
+      <c r="N8" t="inlineStr"/>
+      <c r="O8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>IP</t>
-        </is>
-      </c>
-      <c r="C9" t="n">
-        <v>7</v>
-      </c>
-      <c r="D9" t="n">
-        <v>1</v>
-      </c>
-      <c r="E9" t="n">
-        <v>0</v>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>cifar</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>random</t>
-        </is>
-      </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>SVM</t>
-        </is>
-      </c>
-      <c r="I9" t="inlineStr">
-        <is>
-          <t>['0_0']</t>
-        </is>
-      </c>
-      <c r="J9" t="inlineStr">
-        <is>
-          <t>[100, 133]</t>
-        </is>
-      </c>
-      <c r="K9" t="inlineStr">
-        <is>
-          <t>[0.198, 0.185]</t>
-        </is>
-      </c>
-      <c r="L9" t="inlineStr">
-        <is>
-          <t>[0, 30]</t>
-        </is>
-      </c>
-      <c r="M9" t="inlineStr">
-        <is>
-          <t>[0, 11.899999999999974]</t>
-        </is>
-      </c>
-      <c r="N9" t="inlineStr">
-        <is>
-          <t>[0, 0.2]</t>
-        </is>
-      </c>
-      <c r="O9" t="inlineStr">
-        <is>
-          <t>[-10, -20, 0, -10, -10, 0, -20, 0, 0, -20, 0, 0, -10, -20, 0, -10, -20, 0, 0, -20, 0, -10, 0, 0, 0, -20, -10, 0, -10, 0, -20, 0, -10, -20, -10, 0, -20, 0, 0, -20, 0, -20, 0, 0, -10, 0, -20, 0, 0, 0, 0, -20, -10, 0, -20, -20, -10, -10, 0, 0, -20, -10, 0, -20, -20, -20, 0, 0, -10, 0, 0, -20, 0, -10, -10, -10, -10, -10, -20, 0, 0, -10, 0, 0, -10, 0, 0, 0, -10, -20, 0, -20, 0, 0, 0, -20, -10, 0, 0, 0]</t>
-        </is>
-      </c>
+      <c r="B9" t="inlineStr"/>
+      <c r="C9" t="inlineStr"/>
+      <c r="D9" t="inlineStr"/>
+      <c r="E9" t="inlineStr"/>
+      <c r="F9" t="inlineStr"/>
+      <c r="G9" t="inlineStr"/>
+      <c r="H9" t="inlineStr"/>
+      <c r="I9" t="inlineStr"/>
+      <c r="J9" t="inlineStr"/>
+      <c r="K9" t="inlineStr"/>
+      <c r="L9" t="inlineStr"/>
+      <c r="M9" t="inlineStr"/>
+      <c r="N9" t="inlineStr"/>
+      <c r="O9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>IP</t>
-        </is>
-      </c>
-      <c r="C10" t="n">
-        <v>8</v>
-      </c>
-      <c r="D10" t="n">
-        <v>1</v>
-      </c>
-      <c r="E10" t="n">
-        <v>1</v>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>grocery</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>classWt</t>
-        </is>
-      </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>WVS</t>
-        </is>
-      </c>
-      <c r="I10" t="inlineStr">
-        <is>
-          <t>['5_0']</t>
-        </is>
-      </c>
-      <c r="J10" t="inlineStr">
-        <is>
-          <t>[81, 81]</t>
-        </is>
-      </c>
-      <c r="K10" t="inlineStr">
-        <is>
-          <t>[0.009, 0.009]</t>
-        </is>
-      </c>
-      <c r="L10" t="inlineStr">
-        <is>
-          <t>[0, 30]</t>
-        </is>
-      </c>
-      <c r="M10" t="inlineStr">
-        <is>
-          <t>[0, 12.299999999999972]</t>
-        </is>
-      </c>
-      <c r="N10" t="inlineStr">
-        <is>
-          <t>[0, 0.1]</t>
-        </is>
-      </c>
-      <c r="O10" t="inlineStr">
-        <is>
-          <t>[-10, -10, -10, -10, -10, -10, -10, -10, 0, -10, -10, -10, -10, 0, 0, 0, -10, -20, -20, -20, 0, 0, -20, 0, -20, -20, -20, -20, -20, 0, -20, -20, 0, -20, 0, -20, -20, 0, -20, -20, -10, -20, -20, -10, 0, -20, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, -10, 0, 0, 0, 0, 0, 0, -10, -10, -10, 0, 0, -10, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, -20]</t>
-        </is>
-      </c>
+      <c r="B10" t="inlineStr"/>
+      <c r="C10" t="inlineStr"/>
+      <c r="D10" t="inlineStr"/>
+      <c r="E10" t="inlineStr"/>
+      <c r="F10" t="inlineStr"/>
+      <c r="G10" t="inlineStr"/>
+      <c r="H10" t="inlineStr"/>
+      <c r="I10" t="inlineStr"/>
+      <c r="J10" t="inlineStr"/>
+      <c r="K10" t="inlineStr"/>
+      <c r="L10" t="inlineStr"/>
+      <c r="M10" t="inlineStr"/>
+      <c r="N10" t="inlineStr"/>
+      <c r="O10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">

</xml_diff>